<commit_message>
Update: - Pequeños ajustes al codigo - Cambio de ruta para los ficheros de pruebas acorde a los de OpenBabel
</commit_message>
<xml_diff>
--- a/SMILES_strings.xlsx
+++ b/SMILES_strings.xlsx
@@ -2226,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="83" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update: - Se añaden los archivos relevantes al repositorio de github (tanto los .smi como los .svg resultado)
</commit_message>
<xml_diff>
--- a/SMILES_strings.xlsx
+++ b/SMILES_strings.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="164">
   <si>
     <t>Name</t>
   </si>
@@ -506,13 +506,80 @@
   <si>
     <t>(OC-6-11′)-Bis[2,6-di(2-pyridinyl-κN)phenyl-κC]iron (ACI)
 Otro: Iron, bis[2,6-di(2-pyridinyl-κN)phenyl-κC]-, (OC-6-11′)- (ACI)</t>
+  </si>
+  <si>
+    <t>Diiodo(pentamethylcyclopentadienyl)iridium(III) dimer</t>
+  </si>
+  <si>
+    <t>33040-12-9</t>
+  </si>
+  <si>
+    <t>I[Ir]I.I[Ir]I.C[C]1[C](C)[C](C)[C](C)[C]1C.C[C]2[C](C)[C](C)[C](C)[C]2C</t>
+  </si>
+  <si>
+    <t>[I-][Ir+3]12345([I-][Ir+3]6789([I-])([I-]1)C=%10(C)C9(C)=C8(C)[C-]7(C)C%106C)C=%11(C)C5(C)=C4(C)[C-]3(C)C%112C</t>
+  </si>
+  <si>
+    <t>Ir</t>
+  </si>
+  <si>
+    <t>[Cl-][Ir+3]12345([C-]6=CC(OC)=CC=C6C(=[N]1C=7C=CC(OC)=CC7)C)C=8(C)C5(C)=C4(C)[C-]3(C)C82C</t>
+  </si>
+  <si>
+    <t>[CH]1[CH][CH][CH][CH]1.COc2ccc(cc2)\N=C(/C)c3ccc(OC)cc3[Ir]Cl</t>
+  </si>
+  <si>
+    <r>
+      <t>Chloro[5-methoxy-2-[1-[(4-methoxyphenyl)imino-κ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]ethyl]phenyl-κ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>][(1,2,3,4,5-η)-1,2,3,4,5-pentamethyl-2,4-cyclopentadien-1-yl]iridium (ACI)</t>
+    </r>
+  </si>
+  <si>
+    <t>1258964-48-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -537,6 +604,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FF262626"/>
       <name val="Arial"/>
@@ -570,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -584,6 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1916,6 +1997,94 @@
         <a:xfrm>
           <a:off x="26822400" y="5067300"/>
           <a:ext cx="1080364" cy="774700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>48986</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>141515</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1283693</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1133475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Imagen 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20975411" y="26144765"/>
+          <a:ext cx="1234707" cy="991960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>308882</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1108649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Imagen 32"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21235307" y="26329822"/>
+          <a:ext cx="843643" cy="1108649"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2224,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="83" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="B29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2854,6 +3023,40 @@
       </c>
       <c r="E31" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: - Refactoring de codigo (limpeza de comentarios de debug y algunas traducciones al ingles) - Reorganizacion de carpetas github
</commit_message>
<xml_diff>
--- a/SMILES_strings.xlsx
+++ b/SMILES_strings.xlsx
@@ -2395,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>